<commit_message>
change input source file format from excel to csv, split chiclet output into app versiona and PI.
</commit_message>
<xml_diff>
--- a/Source/target.xlsx
+++ b/Source/target.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangyulin/TVA_filter/Source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangyulin/Desktop/TVA_filter/Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2102DACB-A247-6C44-8471-97EE9925480D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9E9F82-A79B-1945-8146-5FB56F7B6547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1960" windowWidth="16360" windowHeight="16040" xr2:uid="{1B7D0290-52B8-534E-ABA2-AF55B96F8D7E}"/>
+    <workbookView xWindow="14960" yWindow="5300" windowWidth="12200" windowHeight="6780" xr2:uid="{1B7D0290-52B8-534E-ABA2-AF55B96F8D7E}"/>
   </bookViews>
   <sheets>
     <sheet name="target" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>android</t>
   </si>
@@ -42,9 +42,6 @@
     <t>androidTV</t>
   </si>
   <si>
-    <t>chiclet</t>
-  </si>
-  <si>
     <t>fireTV</t>
   </si>
   <si>
@@ -72,7 +69,13 @@
     <t>8.6.182</t>
   </si>
   <si>
-    <t>Playback Hours</t>
+    <t>chiclet-PI</t>
+  </si>
+  <si>
+    <t>chiclet-version</t>
+  </si>
+  <si>
+    <t>8.9.0.36063</t>
   </si>
 </sst>
 </file>
@@ -427,13 +430,14 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -444,54 +448,54 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>20210224</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2">
-        <v>2021</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2">
-        <v>0.51</v>
-      </c>
-      <c r="H2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>